<commit_message>
w3c validating and other corrections as per the advice
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO1.xlsx
+++ b/Modèle-audit-SEO1.xlsx
@@ -187,7 +187,7 @@
     <t xml:space="preserve">de l'élément &lt;label&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">absence de ari-label</t>
+    <t xml:space="preserve">absence de ara-label</t>
   </si>
   <si>
     <t xml:space="preserve">Are label  utilisé pour décrire une structure d'application ou de document, telle que banner, complementary, contentinfo, main, navigation, search</t>
@@ -466,20 +466,19 @@
   </sheetPr>
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1744680851064"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.2893617021277"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.4936170212766"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1914893617021"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.8425531914894"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.7829787234043"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="14.5234042553191"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="9.45957446808511"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9744680851064"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2127659574468"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.7702127659575"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.9617021276596"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.068085106383"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.3872340425532"/>
+    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="15.4255319148936"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>